<commit_message>
Modifications to ensemble scenario stuff and looking into reading heads
</commit_message>
<xml_diff>
--- a/Ensemble_Scenarios.xlsx
+++ b/Ensemble_Scenarios.xlsx
@@ -5,16 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielletadych/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielletadych/Documents/SPRING2020/GroundwaterModelling_HWRS582/FoE_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE3E7560-0572-AB46-BBA3-3C0C4421FC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C51CBE89-0546-F64C-9681-15D5BB11DD2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5620" yWindow="6280" windowWidth="27640" windowHeight="16940" xr2:uid="{34478608-F373-B44C-B24F-CEA82AFF3B9A}"/>
+    <workbookView xWindow="23280" yWindow="5520" windowWidth="25840" windowHeight="16940" xr2:uid="{34478608-F373-B44C-B24F-CEA82AFF3B9A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$11</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="18">
   <si>
     <t>Recharge</t>
   </si>
@@ -74,42 +77,32 @@
     <t>Order</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>High</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> based on sensitivity analysis</t>
-    </r>
+    <t>Reserved?</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Kz top and bottom</t>
+  </si>
+  <si>
+    <t>Specific Y</t>
+  </si>
+  <si>
+    <t>Numbering</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="4">
@@ -148,9 +141,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -166,6 +157,100 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B4BB7F24-C94F-1E43-A8BB-356151BA932D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="495300" y="2425700"/>
+          <a:ext cx="6629400" cy="3352800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Rationale:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>As</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> friends of the Environment, we are concerned with the stream and riparian area.  So we want to run scenarios testing the resliency of both in times of drought.  We also want to investigate the behavior of of the stream and riparian area if the middle layer and Streambed K is altered.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>Our first scenario would be medium and a control.  Then we would conduct a sensitivity analysis by changing all parameters we are interested in to low (Kz top/bottom and Sy would remain medium) and altering one parameter at a time.  We predict ET Valley and ET of the riparian area would have a strong affect on both the riparian area and the stream bed in times of drought (high temperatures = high ET), so some of our scenarios have to do with changing these to high, with low recharge and overrall high ET being the max drought conditions.</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -465,15 +550,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5552713C-B69C-5846-B950-6F9DA9741828}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9:G10"/>
+      <selection activeCell="K2" sqref="K2:K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -481,246 +566,407 @@
         <v>12</v>
       </c>
       <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2">
+        <v>2121331</v>
+      </c>
+      <c r="L2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" s="3">
+        <v>2222222</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="B4">
         <v>8</v>
       </c>
-      <c r="H1" t="s">
+      <c r="C4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K4">
+        <v>2121131</v>
+      </c>
+      <c r="L4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2">
+      <c r="C5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" t="s">
+        <v>5</v>
+      </c>
+      <c r="K5">
+        <v>2121311</v>
+      </c>
+      <c r="L5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
         <v>2</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3">
-        <v>5</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4">
-        <v>6</v>
-      </c>
-      <c r="B4">
+      <c r="C6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" t="s">
+        <v>5</v>
+      </c>
+      <c r="K6">
+        <v>2121111</v>
+      </c>
+      <c r="L6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5">
+      <c r="C7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" t="s">
+        <v>5</v>
+      </c>
+      <c r="H7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I7" t="s">
+        <v>5</v>
+      </c>
+      <c r="K7">
+        <v>2221111</v>
+      </c>
+      <c r="L7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8">
         <v>7</v>
       </c>
-      <c r="B5">
+      <c r="B8">
         <v>4</v>
       </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6">
+      <c r="C8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8" t="s">
+        <v>5</v>
+      </c>
+      <c r="K8">
+        <v>2121121</v>
+      </c>
+      <c r="L8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9">
         <v>8</v>
       </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7">
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" t="s">
+        <v>5</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H9" t="s">
+        <v>5</v>
+      </c>
+      <c r="I9" t="s">
+        <v>5</v>
+      </c>
+      <c r="K9">
+        <v>2121211</v>
+      </c>
+      <c r="L9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10">
         <v>9</v>
       </c>
-      <c r="B7">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F7" t="s">
-        <v>5</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8">
+      <c r="B10">
+        <v>6</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10" t="s">
+        <v>5</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K10">
+        <v>2121112</v>
+      </c>
+      <c r="L10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11">
         <v>10</v>
       </c>
-      <c r="B8">
+      <c r="B11">
         <v>7</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F8" t="s">
-        <v>5</v>
-      </c>
-      <c r="G8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9">
-        <v>3</v>
-      </c>
-      <c r="B9">
-        <v>8</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10">
-        <v>4</v>
-      </c>
-      <c r="B10">
-        <v>9</v>
-      </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11">
-        <v>1</v>
-      </c>
-      <c r="B11">
-        <v>10</v>
-      </c>
-      <c r="C11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F11" t="s">
-        <v>5</v>
+      <c r="C11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="G11" t="s">
         <v>5</v>
       </c>
       <c r="H11" t="s">
-        <v>10</v>
+        <v>5</v>
+      </c>
+      <c r="I11" t="s">
+        <v>5</v>
+      </c>
+      <c r="K11">
+        <v>2122111</v>
+      </c>
+    </row>
+    <row r="24" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E24">
+        <v>1111111</v>
+      </c>
+    </row>
+    <row r="25" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E25">
+        <v>2222222</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="C9:G10"/>
-  </mergeCells>
+  <autoFilter ref="A1:L11" xr:uid="{397D9DDC-A73B-504D-B38E-88CF9407F610}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L11">
+      <sortCondition ref="A1:A11"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>